<commit_message>
Some commit for Partner
</commit_message>
<xml_diff>
--- a/test_data/Выкупы.xlsx
+++ b/test_data/Выкупы.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Astrocatling\WBbot\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1210C7D4-38DC-4A25-AEEB-3745FFF63687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FA74DD-C849-4BE2-B0C3-E45EA275CA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2480" yWindow="1520" windowWidth="28080" windowHeight="15910" xr2:uid="{3D39B954-54E1-433D-BDD4-09D5FB40C627}"/>
+    <workbookView xWindow="960" yWindow="-110" windowWidth="37550" windowHeight="21820" xr2:uid="{3D39B954-54E1-433D-BDD4-09D5FB40C627}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Артикул</t>
   </si>
@@ -46,7 +46,7 @@
     <t>Количество необходимых ПВЗ</t>
   </si>
   <si>
-    <t>пирcинг</t>
+    <t>Пирсинг</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -454,7 +454,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3">
-        <v>63266967</v>
+        <v>63266965</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -468,18 +468,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="3">
-        <v>63266966</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
+      <c r="A3" s="3"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6">

</xml_diff>

<commit_message>
Added for choose tasks
</commit_message>
<xml_diff>
--- a/test_data/Выкупы.xlsx
+++ b/test_data/Выкупы.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Astrocatling\WBbot\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244B42A0-068D-4EBE-A2D1-C5A1AB34015B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A72226-3B7D-4357-8ED1-3CE629EC85B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="-110" windowWidth="37550" windowHeight="21820" xr2:uid="{3D39B954-54E1-433D-BDD4-09D5FB40C627}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Артикул</t>
   </si>
@@ -49,7 +49,10 @@
     <t>Пирсинг</t>
   </si>
   <si>
-    <t>Пирсинг обманка</t>
+    <t>inn</t>
+  </si>
+  <si>
+    <t>312333011857</t>
   </si>
 </sst>
 </file>
@@ -105,13 +108,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -429,7 +433,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -438,6 +442,7 @@
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="11.7265625" customWidth="1"/>
     <col min="4" max="4" width="29.54296875" customWidth="1"/>
+    <col min="5" max="5" width="55.54296875" customWidth="1"/>
     <col min="6" max="6" width="47.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -454,35 +459,29 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3">
-        <v>53597951</v>
+        <v>63266965</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="3">
-        <v>63266965</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6">

</xml_diff>